<commit_message>
arreglos menores e incluir licencia de uso
</commit_message>
<xml_diff>
--- a/FastTest PlugIn - Game.xlsx
+++ b/FastTest PlugIn - Game.xlsx
@@ -24,22 +24,22 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Dificultad</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
-    <t>Pregunta</t>
+    <t>Pregunta / Question</t>
   </si>
   <si>
-    <t>Respuesta 1</t>
+    <t>Respuesta / Answer 1</t>
   </si>
   <si>
-    <t>Respuesta 2</t>
+    <t>Respuesta / Answer 2</t>
   </si>
   <si>
-    <t>Respuesta 3</t>
+    <t>Respuesta / Answer 3</t>
+  </si>
+  <si>
+    <t>Nivel Level</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,6 +157,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +629,7 @@
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -641,27 +647,27 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>1</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="10"/>
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Corrección pequeños errores detectados.
</commit_message>
<xml_diff>
--- a/FastTest PlugIn - Game.xlsx
+++ b/FastTest PlugIn - Game.xlsx
@@ -631,11 +631,11 @@
   <sheetPr codeName="Hoja1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -685,6 +685,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="3">
+        <f>ROW()-2</f>
         <v>1</v>
       </c>
     </row>
@@ -698,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4" si="1">F3+1</f>
+        <f>ROW()-2</f>
         <v>2</v>
       </c>
     </row>
@@ -798,14 +799,6 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
@@ -813,8 +806,9 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>